<commit_message>
added two battery protocols
</commit_message>
<xml_diff>
--- a/Ardentec AGV Data Format.xlsx
+++ b/Ardentec AGV Data Format.xlsx
@@ -1,16 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20385"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107BB1EE-3A7D-48D6-B06B-B932B8835157}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C96F12A-7DDB-4AAE-B19B-61F2D4F7471F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="TCP Protocol" sheetId="1" r:id="rId1"/>
+    <sheet name="舊電池Protocol" sheetId="2" r:id="rId2"/>
+    <sheet name="新電池Protocol" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="208">
   <si>
     <t>Offset</t>
   </si>
@@ -267,6 +270,88 @@
         <family val="1"/>
       </rPr>
       <t xml:space="preserve"> = 0x07</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>normal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> = 0x00
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>emergencyStop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> = 0x01
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>wallDetected</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> = 0x02
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>fenceDetected</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> = 0x03</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -799,84 +884,1470 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>normal</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> = 0x00
+    <t>Communication Parameters</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Baud Rate： 9600 bps
+Data Format：1 start, 8 data, 1 stop, non-parity</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmd  : read data</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC send :</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nomenclature</t>
+  </si>
+  <si>
+    <t>備註</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ex: </t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>FF</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>header</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xFF</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x55</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>EE</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xEE</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>AF</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmd</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xAF</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>battery reply</t>
+  </si>
+  <si>
+    <t>Nomenclature</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>aa</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>0x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>aa</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BMSAlarm</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit7：Over-Temperature Alarm(過溫)
+Bit6：Low SOC Alarm(低SOC)
+Bit5：OverVoltage Alarm(過壓)
+Bit4：UnderTemperture Alarm
+Bit3：Cell UnderVoltage Alarm(欠壓)
+Bit2：OverCurrent Alarm(過流)
+Bit1：ShortCurrent Alarm(短路)
+Bit0：BMS ERROR
 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>emergencyStop</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> += 0x01
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BMSCommand</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit7：Toggle (每讀取一次變化一次)
+Bit6：reserved
+Bit5：Charge Complete Request(停止充電)
+Bit4：reserved
+Bit3：FAN Enable
+Bit2：Full Charge Request(要求長充)
+Bit1：reserved
+Bit0：reserved
 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>wallDetected</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> += 0x02
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>VoltageL</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pack Voltage in mV</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Voltage =VoltageL(0x60)+VoltageH(0x6D)*256=28000 (1mV)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>VoltageH</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOC</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOC in %</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>無號數</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOC : 0~100  (%)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CurrentL</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pack Current in 0.1A</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">有號數 </t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CurrentL=0x38        CurrentH =0xFF 
+CurrentL+(CurrentH&lt;&lt;8)= -200 (10mA)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CurrentH</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BatteryIDL</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery ID</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>無號數</t>
+  </si>
+  <si>
+    <t>BatteryIDL+BatteryIDH*256</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>BatteryIDH</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vcell_MaxL</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max Cell voltage in mV</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>無號數</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>VCell1L(0x1C)+VCell1H(0x0C)*256=3100 (0.1mV)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vcell_MaxH</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vcell_MinL</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Min Cell voltage in mV</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>無號數</t>
+    </r>
+  </si>
+  <si>
+    <t>VCell2L(0x1C)+VCell2H(0x0C)*256=3100 (0.1mV)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vcell_MinH</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tcell_Max</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max Cell Temperature in °C</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>有號數</t>
+    </r>
+  </si>
+  <si>
+    <t>Temperature :  -127 ~127</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tcell_Min</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Min Cell Temperature in °C</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chksum</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Checksum of request </t>
+  </si>
+  <si>
+    <t>chksum方法 :  (chksum之前所有數累加) + chksum = 0</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>起始位址</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>內容</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>資料長度</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>備註</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x0000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Error_Pack_Status</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1word</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>無號數</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2 bytes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Bit 0 = 1 ,batteryID 1 Error
 </t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>fenceDetected</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> += 0x04</t>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Bit 1 = 1 ,batteryID 2 Error
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Bit 2 = 1 ,batteryID 3 Error
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Bit n = 1 ,batteryID (n+1) Error</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x0001</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Voltage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Voltage=Data_H*256 + Data_L
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">= (0x14*256) + 0x1A = 5200
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(uint:10mV)    = 52V</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x0002</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Current</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>有號數</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Current=Data_H*256 + Data_L
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">= (0x01*256) + 0xF4 = 500
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(uint:10mA)    = 5A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x0003</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>SOC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">SOC=Data_H*256 + Data_L
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">= (0x00*256) + 0x4D = 77
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(uint:1%)    = 77%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x0004</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Temp Max</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">T_max=Data_H*256 + Data_L
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">= (0x08*256) + 0x98 = 2200
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(uint:10m℃)    = 22.00℃</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x0005</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Temp Min</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">T_min=Data_H*256 + Data_L
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">= (0x08*256) + 0x34 = 2100
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(uint:10m℃)    = 21.00℃</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x0006</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>CellV Max</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">CellV Max=Data_H*256 + Data_L
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>= (0x8F*256) + 0xFF = 36863 (uint:0.1mV)    = 3.6863V</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x0007</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>CellV Min</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">CellV Min=Data_H*256 + Data_L
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>= (0x8F*256) + 0xFF = 36863 (uint:0.1mV)    = 3.6863V</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x0008</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>CHG_Current</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">CHG_Current=Data_H*256 + Data_L
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">= (0x01*256) + 0xF4 = 500
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(uint:10mA)    = 5A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x0009</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>DSG_Current</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">DSG_Current=Data_H*256 + Data_L
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">= (0x01*256) + 0xF4 = 500
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(uint:10mA)    = 5A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x000A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Basic_Status [0]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>電池基本狀態</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>_LV0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x000B</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Basic_Status [1]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>電池基本狀態</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>_LV1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x000C</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Basic_Status [2]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>電池基本狀態</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>_LV2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x000D</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Extended_Status</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>電池擴展狀態</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x000E</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>SOC_Status</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>電量狀態</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x000F</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Error Code</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>異常代碼</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x0010</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Relay/MOS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Relay/MOS </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>狀態</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x0011</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Cycle</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>循環次數</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x0012</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>FirmwareVersion</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>軟體版本</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>位元</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>項目</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>值</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>範例</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>通訊設備編號</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(1Byte)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x01</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>功能</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(1Byte)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x04</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>起始位置</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(2Byte)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Data_H</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x00</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Data_L</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>資料長度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(2Byte)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x12</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>CRC(2Byte)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x21</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0xC7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>資料長度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(1Byte)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0x24</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>電池資料</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>N-1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>N</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>N+1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>N+2</t>
+    </r>
+  </si>
+  <si>
+    <t>電池單顆資料總覽 (Send)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+      </rPr>
+      <t>電池資料表</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="MingLiU"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve"> (Receive)</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -885,7 +2356,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -931,8 +2402,89 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Microsoft Yi Baiti"/>
+      <family val="4"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="MingLiU"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="MingLiU"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="MingLiU"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="MingLiU"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -963,8 +2515,37 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8CDB3"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -1239,11 +2820,236 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1372,6 +3178,89 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
@@ -1435,9 +3324,166 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="29" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="一般 2" xfId="1" xr:uid="{A4CB4825-6036-4A3B-A091-4419C6D21F7E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1717,11 +3763,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="10.625" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.125" style="2" bestFit="1" customWidth="1"/>
@@ -1731,7 +3777,7 @@
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="19.95" customHeight="1" thickBot="1">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -1742,41 +3788,41 @@
         <v>2</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E1" s="25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="19.95" customHeight="1">
       <c r="A2" s="26">
         <v>0</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="44" t="s">
-        <v>51</v>
+      <c r="C2" s="77" t="s">
+        <v>52</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E2" s="28"/>
     </row>
-    <row r="3" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="19.95" customHeight="1" thickBot="1">
       <c r="A3" s="29">
         <v>1</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="45"/>
+      <c r="C3" s="78"/>
       <c r="D3" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="31"/>
     </row>
-    <row r="4" spans="1:5" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A4" s="22">
         <v>2</v>
       </c>
@@ -1784,14 +3830,14 @@
         <v>6</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="19.95" customHeight="1" thickBot="1">
       <c r="A5" s="19">
         <v>3</v>
       </c>
@@ -1799,14 +3845,14 @@
         <v>12</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D5" s="39"/>
       <c r="E5" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="5" customFormat="1" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="5" customFormat="1" ht="120" customHeight="1" thickBot="1">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -1814,16 +3860,16 @@
         <v>11</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="5" customFormat="1" ht="64.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="5" customFormat="1" ht="64.95" customHeight="1" thickBot="1">
       <c r="A7" s="15">
         <v>5</v>
       </c>
@@ -1831,192 +3877,192 @@
         <v>23</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="5" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="5" customFormat="1" ht="19.95" customHeight="1">
       <c r="A8" s="9">
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="53" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="5" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="83"/>
+      <c r="E8" s="86" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="5" customFormat="1" ht="19.95" customHeight="1">
       <c r="A9" s="11">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="54"/>
-    </row>
-    <row r="10" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="C9" s="90"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="87"/>
+    </row>
+    <row r="10" spans="1:5" ht="19.95" customHeight="1" thickBot="1">
       <c r="A10" s="12">
         <v>8</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="55"/>
-    </row>
-    <row r="11" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C10" s="91"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="88"/>
+    </row>
+    <row r="11" spans="1:5" ht="19.95" customHeight="1">
       <c r="A11" s="14">
         <v>9</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="62"/>
-      <c r="E11" s="59" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="95"/>
+      <c r="E11" s="92" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19.95" customHeight="1">
       <c r="A12" s="11">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="60"/>
-    </row>
-    <row r="13" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="C12" s="90"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="93"/>
+    </row>
+    <row r="13" spans="1:5" ht="19.95" customHeight="1" thickBot="1">
       <c r="A13" s="12">
         <v>11</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="58"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="61"/>
-    </row>
-    <row r="14" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="C13" s="91"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="94"/>
+    </row>
+    <row r="14" spans="1:5" ht="19.95" customHeight="1">
       <c r="A14" s="9">
         <v>12</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="53" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="83"/>
+      <c r="E14" s="86" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="19.95" customHeight="1">
       <c r="A15" s="11">
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="54"/>
-    </row>
-    <row r="16" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="C15" s="81"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="87"/>
+    </row>
+    <row r="16" spans="1:5" ht="19.95" customHeight="1" thickBot="1">
       <c r="A16" s="12">
         <v>14</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="55"/>
-    </row>
-    <row r="17" spans="1:5" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="C16" s="82"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="88"/>
+    </row>
+    <row r="17" spans="1:5" ht="34.950000000000003" customHeight="1" thickBot="1">
       <c r="A17" s="32">
         <v>15</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C17" s="40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E17" s="43" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="19.95" customHeight="1">
       <c r="A18" s="26">
         <v>16</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="44" t="s">
-        <v>52</v>
+      <c r="C18" s="77" t="s">
+        <v>53</v>
       </c>
       <c r="D18" s="37" t="s">
         <v>16</v>
       </c>
       <c r="E18" s="28"/>
     </row>
-    <row r="19" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="19.95" customHeight="1">
       <c r="A19" s="33">
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="46"/>
+      <c r="C19" s="79"/>
       <c r="D19" s="42" t="s">
         <v>17</v>
       </c>
       <c r="E19" s="34"/>
     </row>
-    <row r="20" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="19.95" customHeight="1" thickBot="1">
       <c r="A20" s="29">
         <v>18</v>
       </c>
       <c r="B20" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="45"/>
+      <c r="C20" s="78"/>
       <c r="D20" s="38" t="s">
         <v>18</v>
       </c>
       <c r="E20" s="31"/>
     </row>
-    <row r="21" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="19.95" customHeight="1">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="19.95" customHeight="1">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -2027,7 +4073,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="19.95" customHeight="1">
       <c r="D23" s="1" t="s">
         <v>21</v>
       </c>
@@ -2035,8 +4081,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:5" ht="19.95" customHeight="1"/>
+    <row r="25" spans="1:5" ht="19.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="C2:C3"/>
@@ -2055,4 +4101,1279 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224AB1E1-FA0B-44DD-BB89-C6620DCD33C8}">
+  <dimension ref="B1:G36"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26:F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="2" width="10.875" style="48"/>
+    <col min="3" max="3" width="25.125" style="48" customWidth="1"/>
+    <col min="4" max="4" width="53.625" style="48" customWidth="1"/>
+    <col min="5" max="5" width="48.625" style="48" customWidth="1"/>
+    <col min="6" max="6" width="76.25" style="48" customWidth="1"/>
+    <col min="7" max="7" width="14.875" style="48" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="48"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7">
+      <c r="B1" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="45"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="47"/>
+    </row>
+    <row r="2" spans="2:7">
+      <c r="B2" s="106" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="107"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="49"/>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="109"/>
+      <c r="C3" s="110"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="49"/>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="45"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="50"/>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="53">
+        <v>0</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="50"/>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="53">
+        <v>1</v>
+      </c>
+      <c r="C9" s="54">
+        <v>55</v>
+      </c>
+      <c r="D9" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="50"/>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="53">
+        <v>2</v>
+      </c>
+      <c r="C10" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="50"/>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="53">
+        <v>3</v>
+      </c>
+      <c r="C11" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="50"/>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="53"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="50"/>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="47"/>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="C14" s="58"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="47"/>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="63"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="64">
+        <v>0</v>
+      </c>
+      <c r="C17" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="67"/>
+      <c r="G17" s="63"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="64">
+        <v>1</v>
+      </c>
+      <c r="C18" s="65">
+        <v>55</v>
+      </c>
+      <c r="D18" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="67"/>
+      <c r="G18" s="63"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="64">
+        <v>2</v>
+      </c>
+      <c r="C19" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="67"/>
+      <c r="G19" s="63"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="64">
+        <v>3</v>
+      </c>
+      <c r="C20" s="68">
+        <v>0</v>
+      </c>
+      <c r="D20" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="67"/>
+      <c r="G20" s="63"/>
+    </row>
+    <row r="21" spans="2:7" ht="140.4">
+      <c r="B21" s="64">
+        <v>4</v>
+      </c>
+      <c r="C21" s="69" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="70" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="70"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="63"/>
+    </row>
+    <row r="22" spans="2:7" ht="140.4">
+      <c r="B22" s="64">
+        <v>5</v>
+      </c>
+      <c r="C22" s="71" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="72" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="72"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="63"/>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="64">
+        <v>6</v>
+      </c>
+      <c r="C23" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="104" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="112"/>
+      <c r="F23" s="113" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="63"/>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="64">
+        <v>7</v>
+      </c>
+      <c r="C24" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="105"/>
+      <c r="E24" s="105"/>
+      <c r="F24" s="114"/>
+      <c r="G24" s="63"/>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="64">
+        <v>8</v>
+      </c>
+      <c r="C25" s="65" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" s="67" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="63"/>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="64">
+        <v>9</v>
+      </c>
+      <c r="C26" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" s="104" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="104" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="115" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" s="63"/>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="64">
+        <v>10</v>
+      </c>
+      <c r="C27" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="105"/>
+      <c r="E27" s="105"/>
+      <c r="F27" s="116"/>
+      <c r="G27" s="63"/>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="64">
+        <v>11</v>
+      </c>
+      <c r="C28" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="104" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="104" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28" s="102" t="s">
+        <v>94</v>
+      </c>
+      <c r="G28" s="63"/>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="64">
+        <v>12</v>
+      </c>
+      <c r="C29" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="105"/>
+      <c r="E29" s="105"/>
+      <c r="F29" s="103"/>
+      <c r="G29" s="63"/>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="64">
+        <v>13</v>
+      </c>
+      <c r="C30" s="65" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="98" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" s="100" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" s="102" t="s">
+        <v>99</v>
+      </c>
+      <c r="G30" s="63"/>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" s="64">
+        <v>14</v>
+      </c>
+      <c r="C31" s="65" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" s="99"/>
+      <c r="E31" s="101"/>
+      <c r="F31" s="103"/>
+      <c r="G31" s="63"/>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" s="64">
+        <v>15</v>
+      </c>
+      <c r="C32" s="65" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="98" t="s">
+        <v>102</v>
+      </c>
+      <c r="E32" s="100" t="s">
+        <v>103</v>
+      </c>
+      <c r="F32" s="102" t="s">
+        <v>104</v>
+      </c>
+      <c r="G32" s="63"/>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="64">
+        <v>16</v>
+      </c>
+      <c r="C33" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="99"/>
+      <c r="E33" s="101"/>
+      <c r="F33" s="103"/>
+      <c r="G33" s="63"/>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" s="64">
+        <v>17</v>
+      </c>
+      <c r="C34" s="65" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34" s="66" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34" s="74" t="s">
+        <v>108</v>
+      </c>
+      <c r="F34" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="G34" s="63"/>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35" s="64">
+        <v>18</v>
+      </c>
+      <c r="C35" s="65" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="66" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" s="74" t="s">
+        <v>108</v>
+      </c>
+      <c r="F35" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="G35" s="63"/>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" s="64">
+        <v>19</v>
+      </c>
+      <c r="C36" s="76" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36" s="66"/>
+      <c r="F36" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="G36" s="63"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7F738E-E838-4929-8DD1-0EF1DB6F9CB1}">
+  <dimension ref="A1:N23"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="19.25" customWidth="1"/>
+    <col min="3" max="3" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.5" customWidth="1"/>
+    <col min="9" max="9" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9" customWidth="1"/>
+    <col min="12" max="12" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.125" customWidth="1"/>
+    <col min="14" max="14" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="19.8">
+      <c r="A1" s="149" t="s">
+        <v>207</v>
+      </c>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="118"/>
+      <c r="I1" s="148" t="s">
+        <v>206</v>
+      </c>
+      <c r="J1" s="128"/>
+      <c r="K1" s="128"/>
+      <c r="L1" s="128"/>
+      <c r="M1" s="128"/>
+      <c r="N1" s="127"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="120" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="120" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="120" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="120" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="117"/>
+      <c r="I2" s="120" t="s">
+        <v>180</v>
+      </c>
+      <c r="J2" s="129" t="s">
+        <v>181</v>
+      </c>
+      <c r="K2" s="130"/>
+      <c r="L2" s="120" t="s">
+        <v>182</v>
+      </c>
+      <c r="M2" s="120" t="s">
+        <v>183</v>
+      </c>
+      <c r="N2" s="117"/>
+    </row>
+    <row r="3" spans="1:14" ht="55.2">
+      <c r="A3" s="122" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="122" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="122" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="126" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="122" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" s="123" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" s="117"/>
+      <c r="I3" s="131">
+        <v>0</v>
+      </c>
+      <c r="J3" s="132" t="s">
+        <v>184</v>
+      </c>
+      <c r="K3" s="133"/>
+      <c r="L3" s="124" t="s">
+        <v>185</v>
+      </c>
+      <c r="M3" s="124" t="s">
+        <v>186</v>
+      </c>
+      <c r="N3" s="117"/>
+    </row>
+    <row r="4" spans="1:14" ht="41.4">
+      <c r="A4" s="122" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="122" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="122" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="126" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="122" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" s="123" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" s="117"/>
+      <c r="I4" s="131">
+        <v>1</v>
+      </c>
+      <c r="J4" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="K4" s="133"/>
+      <c r="L4" s="124" t="s">
+        <v>185</v>
+      </c>
+      <c r="M4" s="124" t="s">
+        <v>188</v>
+      </c>
+      <c r="N4" s="117"/>
+    </row>
+    <row r="5" spans="1:14" ht="41.4">
+      <c r="A5" s="122" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="122" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="122" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="126" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="122" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="123" t="s">
+        <v>131</v>
+      </c>
+      <c r="G5" s="117"/>
+      <c r="I5" s="131">
+        <v>2</v>
+      </c>
+      <c r="J5" s="134" t="s">
+        <v>189</v>
+      </c>
+      <c r="K5" s="135"/>
+      <c r="L5" s="124" t="s">
+        <v>190</v>
+      </c>
+      <c r="M5" s="124" t="s">
+        <v>191</v>
+      </c>
+      <c r="N5" s="117"/>
+    </row>
+    <row r="6" spans="1:14" ht="41.4">
+      <c r="A6" s="122" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="122" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="122" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="126" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="122" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" s="123" t="s">
+        <v>134</v>
+      </c>
+      <c r="G6" s="117"/>
+      <c r="I6" s="131">
+        <v>3</v>
+      </c>
+      <c r="J6" s="136"/>
+      <c r="K6" s="137"/>
+      <c r="L6" s="124" t="s">
+        <v>192</v>
+      </c>
+      <c r="M6" s="124" t="s">
+        <v>186</v>
+      </c>
+      <c r="N6" s="117"/>
+    </row>
+    <row r="7" spans="1:14" ht="41.4">
+      <c r="A7" s="124" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="124" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" s="124" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="120" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="124" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" s="125" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" s="117"/>
+      <c r="I7" s="131">
+        <v>4</v>
+      </c>
+      <c r="J7" s="134" t="s">
+        <v>193</v>
+      </c>
+      <c r="K7" s="135"/>
+      <c r="L7" s="124" t="s">
+        <v>190</v>
+      </c>
+      <c r="M7" s="124" t="s">
+        <v>191</v>
+      </c>
+      <c r="N7" s="117"/>
+    </row>
+    <row r="8" spans="1:14" ht="41.4">
+      <c r="A8" s="124" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="124" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="124" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="120" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="124" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" s="125" t="s">
+        <v>140</v>
+      </c>
+      <c r="G8" s="117"/>
+      <c r="I8" s="131">
+        <v>5</v>
+      </c>
+      <c r="J8" s="136"/>
+      <c r="K8" s="137"/>
+      <c r="L8" s="124" t="s">
+        <v>192</v>
+      </c>
+      <c r="M8" s="124" t="s">
+        <v>194</v>
+      </c>
+      <c r="N8" s="117"/>
+    </row>
+    <row r="9" spans="1:14" ht="41.4">
+      <c r="A9" s="124" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" s="124" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="124" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" s="120" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="124" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" s="125" t="s">
+        <v>143</v>
+      </c>
+      <c r="G9" s="117"/>
+      <c r="I9" s="131">
+        <v>6</v>
+      </c>
+      <c r="J9" s="138" t="s">
+        <v>195</v>
+      </c>
+      <c r="K9" s="139"/>
+      <c r="L9" s="124" t="s">
+        <v>192</v>
+      </c>
+      <c r="M9" s="124" t="s">
+        <v>196</v>
+      </c>
+      <c r="N9" s="117"/>
+    </row>
+    <row r="10" spans="1:14" ht="41.4">
+      <c r="A10" s="124" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="124" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="124" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="120" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="124" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="125" t="s">
+        <v>146</v>
+      </c>
+      <c r="G10" s="117"/>
+      <c r="I10" s="131">
+        <v>7</v>
+      </c>
+      <c r="J10" s="140"/>
+      <c r="K10" s="141"/>
+      <c r="L10" s="124" t="s">
+        <v>190</v>
+      </c>
+      <c r="M10" s="124" t="s">
+        <v>197</v>
+      </c>
+      <c r="N10" s="117"/>
+    </row>
+    <row r="11" spans="1:14" ht="41.4">
+      <c r="A11" s="124" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="124" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="124" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="120" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" s="124" t="s">
+        <v>123</v>
+      </c>
+      <c r="F11" s="125" t="s">
+        <v>149</v>
+      </c>
+      <c r="G11" s="117"/>
+      <c r="I11" s="120" t="s">
+        <v>180</v>
+      </c>
+      <c r="J11" s="129" t="s">
+        <v>181</v>
+      </c>
+      <c r="K11" s="130"/>
+      <c r="L11" s="120" t="s">
+        <v>182</v>
+      </c>
+      <c r="M11" s="120" t="s">
+        <v>183</v>
+      </c>
+      <c r="N11" s="117"/>
+    </row>
+    <row r="12" spans="1:14" ht="41.4">
+      <c r="A12" s="124" t="s">
+        <v>150</v>
+      </c>
+      <c r="B12" s="124" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="124" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="120" t="s">
+        <v>130</v>
+      </c>
+      <c r="E12" s="124" t="s">
+        <v>123</v>
+      </c>
+      <c r="F12" s="125" t="s">
+        <v>152</v>
+      </c>
+      <c r="G12" s="117"/>
+      <c r="I12" s="131">
+        <v>0</v>
+      </c>
+      <c r="J12" s="132" t="s">
+        <v>184</v>
+      </c>
+      <c r="K12" s="133"/>
+      <c r="L12" s="124" t="s">
+        <v>185</v>
+      </c>
+      <c r="M12" s="124" t="s">
+        <v>186</v>
+      </c>
+      <c r="N12" s="117"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="124" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" s="124" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="124" t="s">
+        <v>121</v>
+      </c>
+      <c r="D13" s="120" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" s="124" t="s">
+        <v>123</v>
+      </c>
+      <c r="F13" s="125" t="s">
+        <v>155</v>
+      </c>
+      <c r="G13" s="117"/>
+      <c r="I13" s="131">
+        <v>1</v>
+      </c>
+      <c r="J13" s="132" t="s">
+        <v>187</v>
+      </c>
+      <c r="K13" s="133"/>
+      <c r="L13" s="124" t="s">
+        <v>185</v>
+      </c>
+      <c r="M13" s="124" t="s">
+        <v>188</v>
+      </c>
+      <c r="N13" s="117"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="124" t="s">
+        <v>156</v>
+      </c>
+      <c r="B14" s="124" t="s">
+        <v>157</v>
+      </c>
+      <c r="C14" s="124" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="120" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14" s="124" t="s">
+        <v>123</v>
+      </c>
+      <c r="F14" s="125" t="s">
+        <v>158</v>
+      </c>
+      <c r="G14" s="117"/>
+      <c r="I14" s="131">
+        <v>2</v>
+      </c>
+      <c r="J14" s="132" t="s">
+        <v>198</v>
+      </c>
+      <c r="K14" s="133"/>
+      <c r="L14" s="124" t="s">
+        <v>185</v>
+      </c>
+      <c r="M14" s="124" t="s">
+        <v>199</v>
+      </c>
+      <c r="N14" s="117"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="124" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="124" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15" s="124" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="120" t="s">
+        <v>122</v>
+      </c>
+      <c r="E15" s="124" t="s">
+        <v>123</v>
+      </c>
+      <c r="F15" s="125" t="s">
+        <v>161</v>
+      </c>
+      <c r="G15" s="117"/>
+      <c r="I15" s="131">
+        <v>3</v>
+      </c>
+      <c r="J15" s="142" t="s">
+        <v>200</v>
+      </c>
+      <c r="K15" s="143"/>
+      <c r="L15" s="124" t="s">
+        <v>190</v>
+      </c>
+      <c r="M15" s="121"/>
+      <c r="N15" s="117"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="124" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" s="124" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" s="124" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="120" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" s="124" t="s">
+        <v>123</v>
+      </c>
+      <c r="F16" s="120" t="s">
+        <v>164</v>
+      </c>
+      <c r="G16" s="117"/>
+      <c r="I16" s="131">
+        <v>4</v>
+      </c>
+      <c r="J16" s="144"/>
+      <c r="K16" s="145"/>
+      <c r="L16" s="124" t="s">
+        <v>192</v>
+      </c>
+      <c r="M16" s="121"/>
+      <c r="N16" s="117"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="124" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" s="124" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" s="124" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="120" t="s">
+        <v>122</v>
+      </c>
+      <c r="E17" s="124" t="s">
+        <v>123</v>
+      </c>
+      <c r="F17" s="120" t="s">
+        <v>167</v>
+      </c>
+      <c r="G17" s="117"/>
+      <c r="I17" s="131">
+        <v>5</v>
+      </c>
+      <c r="J17" s="144"/>
+      <c r="K17" s="145"/>
+      <c r="L17" s="124" t="s">
+        <v>190</v>
+      </c>
+      <c r="M17" s="121"/>
+      <c r="N17" s="117"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="124" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" s="124" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" s="124" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="120" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" s="124" t="s">
+        <v>123</v>
+      </c>
+      <c r="F18" s="120" t="s">
+        <v>170</v>
+      </c>
+      <c r="G18" s="117"/>
+      <c r="I18" s="131">
+        <v>6</v>
+      </c>
+      <c r="J18" s="144"/>
+      <c r="K18" s="145"/>
+      <c r="L18" s="124" t="s">
+        <v>192</v>
+      </c>
+      <c r="M18" s="121"/>
+      <c r="N18" s="117"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="124" t="s">
+        <v>171</v>
+      </c>
+      <c r="B19" s="124" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="124" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="120" t="s">
+        <v>122</v>
+      </c>
+      <c r="E19" s="124" t="s">
+        <v>123</v>
+      </c>
+      <c r="F19" s="125" t="s">
+        <v>173</v>
+      </c>
+      <c r="G19" s="117"/>
+      <c r="I19" s="124" t="s">
+        <v>201</v>
+      </c>
+      <c r="J19" s="144"/>
+      <c r="K19" s="145"/>
+      <c r="L19" s="124" t="s">
+        <v>201</v>
+      </c>
+      <c r="M19" s="121"/>
+      <c r="N19" s="117"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="124" t="s">
+        <v>174</v>
+      </c>
+      <c r="B20" s="124" t="s">
+        <v>175</v>
+      </c>
+      <c r="C20" s="124" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="120" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="124" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" s="120" t="s">
+        <v>176</v>
+      </c>
+      <c r="G20" s="117"/>
+      <c r="I20" s="124" t="s">
+        <v>202</v>
+      </c>
+      <c r="J20" s="144"/>
+      <c r="K20" s="145"/>
+      <c r="L20" s="124" t="s">
+        <v>190</v>
+      </c>
+      <c r="M20" s="121"/>
+      <c r="N20" s="117"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="B21" s="124" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" s="124" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="120" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="124" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" s="120" t="s">
+        <v>179</v>
+      </c>
+      <c r="G21" s="117"/>
+      <c r="I21" s="124" t="s">
+        <v>203</v>
+      </c>
+      <c r="J21" s="146"/>
+      <c r="K21" s="147"/>
+      <c r="L21" s="124" t="s">
+        <v>192</v>
+      </c>
+      <c r="M21" s="121"/>
+      <c r="N21" s="117"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="I22" s="124" t="s">
+        <v>204</v>
+      </c>
+      <c r="J22" s="138" t="s">
+        <v>195</v>
+      </c>
+      <c r="K22" s="139"/>
+      <c r="L22" s="124" t="s">
+        <v>192</v>
+      </c>
+      <c r="M22" s="121"/>
+      <c r="N22" s="117"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="I23" s="124" t="s">
+        <v>205</v>
+      </c>
+      <c r="J23" s="140"/>
+      <c r="K23" s="141"/>
+      <c r="L23" s="124" t="s">
+        <v>190</v>
+      </c>
+      <c r="M23" s="121"/>
+      <c r="N23" s="117"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K21"/>
+    <mergeCell ref="J22:K23"/>
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="J7:K8"/>
+    <mergeCell ref="J9:K10"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J3:K3"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>